<commit_message>
add Appunti di Core Java e .gitignore
</commit_message>
<xml_diff>
--- a/Shortcuts.xlsx
+++ b/Shortcuts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="512">
   <si>
     <t xml:space="preserve">gJgz^*RTtk^3*e56N#66*9^t%#6*SMY95HNTj^bh4*2RS$4mzfpim4</t>
   </si>
@@ -2016,6 +2016,12 @@
   </si>
   <si>
     <t xml:space="preserve">git push -u remote_name branch // git push -u remote_name local_branch:remote_branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push su repo GitHub che è obbligata ad aggiornarsi (non usare in caso di pull altrui)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git push -f remote_name branch</t>
   </si>
   <si>
     <t xml:space="preserve">Passo localmente a branch con stesso nome del remote, settando collegamento tra i 2</t>
@@ -2666,7 +2672,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2723,14 +2729,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2754,7 +2752,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.89"/>
   </cols>
@@ -2795,106 +2793,106 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2933,34 +2931,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2988,7 +2986,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="67.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="96.63"/>
@@ -2996,23 +2994,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>198</v>
@@ -3052,10 +3050,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -3089,10 +3087,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -7528,7 +7526,7 @@
       <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="134.95"/>
@@ -8456,8 +8454,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B86" activeCellId="0" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9089,22 +9087,22 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="2"/>
+      <c r="A83" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>311</v>
-      </c>
+      <c r="B84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>396</v>
+        <v>310</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>397</v>
+        <v>311</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9147,11 +9145,11 @@
         <v>407</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>409</v>
       </c>
     </row>
@@ -9180,15 +9178,15 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="2"/>
+      <c r="A96" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>417</v>
-      </c>
+      <c r="B97" s="2"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
@@ -9271,15 +9269,15 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="2"/>
+      <c r="A108" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>439</v>
-      </c>
+      <c r="B109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
@@ -9298,48 +9296,48 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="2"/>
+      <c r="A112" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="2" t="s">
-        <v>444</v>
-      </c>
       <c r="B113" s="2"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="B114" s="15" t="s">
+      <c r="A114" s="2" t="s">
         <v>446</v>
       </c>
+      <c r="B114" s="2"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="14" t="s">
+      <c r="A115" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="B115" s="15" t="s">
+      <c r="B115" s="2" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="14" t="s">
+      <c r="A116" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="B116" s="15" t="s">
+      <c r="B116" s="2" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="2"/>
+      <c r="A117" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>452</v>
-      </c>
+      <c r="B118" s="2"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
@@ -9397,7 +9395,14 @@
         <v>466</v>
       </c>
     </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Cap. 1 e 2
</commit_message>
<xml_diff>
--- a/Shortcuts.xlsx
+++ b/Shortcuts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="516">
   <si>
     <t xml:space="preserve">gJgz^*RTtk^3*e56N#66*9^t%#6*SMY95HNTj^bh4*2RS$4mzfpim4</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t xml:space="preserve">mouse su barra applicazioni → impostazioni della barra applicazioni → comportamenti della barra applicazioni → nascondi automaticamente barra applicazioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizza estensioni dei files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start → Esplora file → Visualizza → Mostra → “Estensione nomi file”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizza files nascosti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start → Esplora file → Visualizza → Mostra → “Elementi nascosti”</t>
   </si>
   <si>
     <t xml:space="preserve">Formattazione automatica</t>
@@ -700,6 +712,12 @@
   </si>
   <si>
     <t xml:space="preserve">command palettee → digito Markdown open preview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check updates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click in alto a sin → guida → controlla disponibilità aggiornamenti</t>
   </si>
   <si>
     <t xml:space="preserve">Aprire "Strumenti per Sviluppatori"</t>
@@ -2666,7 +2684,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2703,8 +2721,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2720,14 +2750,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2754,7 +2776,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.89"/>
   </cols>
@@ -2795,106 +2817,106 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2933,34 +2955,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2988,7 +3010,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="67.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="96.63"/>
@@ -2996,26 +3018,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3052,10 +3074,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -3089,10 +3111,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -3177,10 +3199,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3236,6 +3258,22 @@
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3269,135 +3307,135 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3405,63 +3443,63 @@
         <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3470,15 +3508,15 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B28" s="4"/>
     </row>
@@ -3496,18 +3534,18 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7528,7 +7566,7 @@
       <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="134.95"/>
@@ -7536,421 +7574,421 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
       <c r="B41" s="7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>
       <c r="B42" s="7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7"/>
       <c r="B44" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7"/>
       <c r="B45" s="7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B56" s="7"/>
     </row>
@@ -7970,10 +8008,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7985,186 +8023,194 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>160</v>
+      <c r="A3" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>162</v>
+      <c r="A4" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>164</v>
+      <c r="A5" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>166</v>
+      <c r="A6" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>168</v>
+      <c r="A7" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>170</v>
+      <c r="A8" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>172</v>
+      <c r="A9" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>174</v>
+      <c r="A10" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>175</v>
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>177</v>
+      <c r="A12" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>179</v>
+      <c r="A13" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>181</v>
+      <c r="A14" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>183</v>
+      <c r="A15" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>185</v>
+      <c r="A16" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>188</v>
+      <c r="A18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>190</v>
+      <c r="A19" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>192</v>
+      <c r="A20" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>194</v>
+      <c r="A21" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>196</v>
+      <c r="A22" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>198</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -8186,7 +8232,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8198,31 +8244,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -8256,186 +8302,186 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -8456,8 +8502,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8469,256 +8515,256 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>282</v>
+        <v>287</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>284</v>
+        <v>289</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8727,90 +8773,90 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>327</v>
+        <v>332</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8819,50 +8865,50 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8870,222 +8916,222 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>355</v>
+      <c r="A60" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="12"/>
-      <c r="B61" s="13"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="16"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>357</v>
+      <c r="A62" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>359</v>
+      <c r="A63" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>361</v>
+      <c r="A64" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>363</v>
+      <c r="A65" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>365</v>
+      <c r="A66" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>367</v>
+      <c r="A67" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9093,90 +9139,90 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9184,90 +9230,90 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9275,26 +9321,26 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9302,32 +9348,32 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="B113" s="2"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>446</v>
+      <c r="A114" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>448</v>
+      <c r="A115" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="14" t="s">
-        <v>449</v>
-      </c>
-      <c r="B116" s="15" t="s">
-        <v>450</v>
+      <c r="A116" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9335,66 +9381,66 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>452</v>
+        <v>457</v>
+      </c>
+      <c r="B118" s="11" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>454</v>
+        <v>459</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>456</v>
+        <v>461</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>458</v>
+        <v>463</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>460</v>
+        <v>465</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>462</v>
+        <v>467</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="B124" s="9" t="s">
-        <v>464</v>
+        <v>469</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>466</v>
+        <v>471</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>